<commit_message>
updated api code for new dga tool version 3.0.1
</commit_message>
<xml_diff>
--- a/api/tests/single_trafo.xlsx
+++ b/api/tests/single_trafo.xlsx
@@ -674,11 +674,11 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2:W18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.11"/>
@@ -694,7 +694,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="8.11"/>
@@ -787,7 +787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>28</v>
       </c>
@@ -851,6 +851,12 @@
       <c r="U2" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="V2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X2" s="0" t="s">
         <v>44</v>
       </c>
@@ -867,7 +873,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>49</v>
       </c>
@@ -931,6 +937,12 @@
       <c r="U3" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="V3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X3" s="0" t="s">
         <v>57</v>
       </c>
@@ -944,7 +956,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>61</v>
       </c>
@@ -1008,6 +1020,12 @@
       <c r="U4" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="V4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X4" s="0" t="s">
         <v>68</v>
       </c>
@@ -1021,7 +1039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>71</v>
       </c>
@@ -1085,6 +1103,12 @@
       <c r="U5" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="V5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X5" s="0" t="s">
         <v>57</v>
       </c>
@@ -1098,7 +1122,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>78</v>
       </c>
@@ -1162,6 +1186,12 @@
       <c r="U6" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="V6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X6" s="0" t="s">
         <v>57</v>
       </c>
@@ -1175,7 +1205,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>86</v>
       </c>
@@ -1239,6 +1269,12 @@
       <c r="U7" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="V7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X7" s="0" t="s">
         <v>57</v>
       </c>
@@ -1252,7 +1288,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>94</v>
       </c>
@@ -1316,6 +1352,12 @@
       <c r="U8" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="V8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X8" s="0" t="s">
         <v>100</v>
       </c>
@@ -1329,7 +1371,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>103</v>
       </c>
@@ -1393,6 +1435,12 @@
       <c r="U9" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="V9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X9" s="0" t="s">
         <v>109</v>
       </c>
@@ -1406,7 +1454,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>112</v>
       </c>
@@ -1469,6 +1517,12 @@
       </c>
       <c r="U10" s="0" t="s">
         <v>29</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="X10" s="0" t="s">
         <v>117</v>
@@ -1547,6 +1601,12 @@
       <c r="U11" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="V11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X11" s="0" t="s">
         <v>126</v>
       </c>
@@ -1627,6 +1687,12 @@
       <c r="U12" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="V12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X12" s="0" t="s">
         <v>134</v>
       </c>
@@ -1643,7 +1709,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>138</v>
       </c>
@@ -1707,6 +1773,12 @@
       <c r="U13" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="V13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X13" s="0" t="s">
         <v>142</v>
       </c>
@@ -1720,7 +1792,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>145</v>
       </c>
@@ -1784,6 +1856,12 @@
       <c r="U14" s="0" t="s">
         <v>151</v>
       </c>
+      <c r="V14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X14" s="0" t="s">
         <v>152</v>
       </c>
@@ -1800,7 +1878,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>156</v>
       </c>
@@ -1864,6 +1942,12 @@
       <c r="U15" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="V15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X15" s="0" t="s">
         <v>127</v>
       </c>
@@ -1880,7 +1964,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>164</v>
       </c>
@@ -1944,6 +2028,12 @@
       <c r="U16" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="V16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X16" s="0" t="s">
         <v>168</v>
       </c>
@@ -1957,7 +2047,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>172</v>
       </c>
@@ -2021,6 +2111,12 @@
       <c r="U17" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="V17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="X17" s="0" t="s">
         <v>134</v>
       </c>
@@ -2034,7 +2130,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>178</v>
       </c>
@@ -2097,6 +2193,12 @@
       </c>
       <c r="U18" s="0" t="s">
         <v>29</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="X18" s="0" t="s">
         <v>181</v>

</xml_diff>